<commit_message>
Practica 12 y Calificaciones Parcial 1 y 2
</commit_message>
<xml_diff>
--- a/Parcial2.xlsx
+++ b/Parcial2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Universidad_Panamerica\2026-1\Analisis_y_diseño_de_Algoritmos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Universidad_Panamerica\2026-1\Analisis_y_diseño_de_Algoritmos\Curso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D912DAE-0660-43BF-A426-DF1F9E4C357A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B03B16-F682-4505-A0D0-6EA73FC24B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14657" yWindow="0" windowWidth="14914" windowHeight="11709" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36540" yWindow="2450" windowWidth="14670" windowHeight="8480" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Practica9" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -414,13 +414,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,22 +1084,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -1737,10 +1736,10 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14:K15"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1811,28 +1810,28 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="14">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14">
+      <c r="G2" s="13">
+        <v>0.82857142857142851</v>
+      </c>
+      <c r="H2" s="13">
         <v>0.7</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="13">
         <v>0.55999999999999994</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="13">
         <v>0.5</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="13">
         <v>0.95000000000000007</v>
       </c>
       <c r="L2">
@@ -1843,7 +1842,7 @@
       </c>
       <c r="N2">
         <f>(SUM(D2:K3)+L2)*0.6/9+M2*0.4</f>
-        <v>0.76288888888888895</v>
+        <v>0.81812698412698415</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -1856,14 +1855,14 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
       <c r="L3">
         <v>0.80000000000000016</v>
       </c>
@@ -1872,7 +1871,7 @@
       </c>
       <c r="N3">
         <f>(SUM(D2:K3)+L3)*0.6/9+M3*0.4</f>
-        <v>0.6651111111111111</v>
+        <v>0.72034920634920641</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
@@ -1885,28 +1884,28 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="14">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14">
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
         <v>0.6333333333333333</v>
       </c>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
         <v>0.67999999999999994</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <v>0.96</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>0.95</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>1</v>
       </c>
       <c r="L4">
@@ -1930,14 +1929,14 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
       <c r="L5">
         <v>1</v>
       </c>
@@ -1959,28 +1958,28 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>0.5</v>
       </c>
-      <c r="E6" s="14">
-        <v>1</v>
-      </c>
-      <c r="F6" s="14">
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
         <v>0.79999999999999993</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>0.5714285714285714</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>0.82</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <v>0.6</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>0.95</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>0</v>
       </c>
       <c r="L6">
@@ -2004,14 +2003,14 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
       <c r="L7">
         <v>0.9</v>
       </c>
@@ -2033,28 +2032,28 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
         <v>0.93333333333333324</v>
       </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
         <v>0.6</v>
       </c>
-      <c r="J8" s="14">
-        <v>1</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
         <v>1</v>
       </c>
       <c r="L8">
@@ -2078,14 +2077,14 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
       <c r="L9">
         <v>1</v>
       </c>
@@ -2107,28 +2106,28 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
         <v>0.72000000000000008</v>
       </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="14">
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13">
         <v>0.95</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <v>1</v>
       </c>
       <c r="L10">
@@ -2152,14 +2151,14 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
       <c r="L11">
         <v>0.96666666666666667</v>
       </c>
@@ -2181,28 +2180,28 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>0.53333333333333333</v>
       </c>
-      <c r="E12" s="14">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
         <v>0.39999999999999997</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>0.5714285714285714</v>
       </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
         <v>0.5</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <v>0.64999999999999991</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="13">
         <v>0.33333333333333331</v>
       </c>
       <c r="L12">
@@ -2226,14 +2225,14 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
       <c r="L13">
         <v>1</v>
       </c>
@@ -2255,28 +2254,28 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
         <v>0.16666666666666666</v>
       </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
         <v>0</v>
       </c>
       <c r="L14">
@@ -2291,26 +2290,53 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
@@ -2323,42 +2349,14 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2417,25 +2415,25 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>0.7</v>
       </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14">
-        <v>1</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14">
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
         <f>(SUM(D2:I3))/6</f>
         <v>0.95000000000000007</v>
       </c>
@@ -2450,13 +2448,13 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -2468,25 +2466,25 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14">
-        <v>1</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
         <f>(SUM(D4:I5))/6</f>
         <v>1</v>
       </c>
@@ -2501,13 +2499,13 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -2519,25 +2517,25 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="14">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
         <f>(SUM(D6:I7))/6</f>
         <v>0</v>
       </c>
@@ -2552,13 +2550,13 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -2570,25 +2568,25 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>1</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="14">
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
         <f>(SUM(D8:I9))/6</f>
         <v>1</v>
       </c>
@@ -2603,13 +2601,13 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -2621,25 +2619,25 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="14">
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13">
         <f>(SUM(D10:I11))/6</f>
         <v>1</v>
       </c>
@@ -2654,13 +2652,13 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -2672,25 +2670,25 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
         <f>(SUM(D12:I13))/6</f>
         <v>0.33333333333333331</v>
       </c>
@@ -2705,13 +2703,13 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -2723,60 +2721,53 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="13">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
         <f>(SUM(D14:I15))/6</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="J4:J5"/>
@@ -2793,19 +2784,26 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2857,19 +2855,19 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14">
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13">
         <f>(SUM(D2:G3))/4</f>
         <v>0.5</v>
       </c>
@@ -2884,11 +2882,11 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -2900,20 +2898,20 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14">
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13">
         <v>0.8</v>
       </c>
-      <c r="H4" s="14">
-        <f t="shared" ref="H4:H15" si="0">(SUM(D4:G5))/4</f>
+      <c r="H4" s="13">
+        <f t="shared" ref="H4" si="0">(SUM(D4:G5))/4</f>
         <v>0.95</v>
       </c>
     </row>
@@ -2927,11 +2925,11 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -2943,20 +2941,20 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="14">
         <v>0.9</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>0.9</v>
       </c>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14">
-        <f t="shared" ref="H6:H15" si="1">(SUM(D6:G7))/4</f>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" ref="H6" si="1">(SUM(D6:G7))/4</f>
         <v>0.95</v>
       </c>
     </row>
@@ -2970,11 +2968,11 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -2986,20 +2984,20 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>1</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <f t="shared" ref="H8:H15" si="2">(SUM(D8:G9))/4</f>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" ref="H8" si="2">(SUM(D8:G9))/4</f>
         <v>1</v>
       </c>
     </row>
@@ -3013,11 +3011,11 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -3029,20 +3027,20 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
         <v>0.9</v>
       </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
         <v>0.9</v>
       </c>
-      <c r="H10" s="14">
-        <f t="shared" ref="H10:H15" si="3">(SUM(D10:G11))/4</f>
+      <c r="H10" s="13">
+        <f t="shared" ref="H10" si="3">(SUM(D10:G11))/4</f>
         <v>0.95</v>
       </c>
     </row>
@@ -3056,11 +3054,11 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -3072,20 +3070,20 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>0.7</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>0.5</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>0.7</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>0.7</v>
       </c>
-      <c r="H12" s="14">
-        <f t="shared" ref="H12:H15" si="4">(SUM(D12:G13))/4</f>
+      <c r="H12" s="13">
+        <f t="shared" ref="H12" si="4">(SUM(D12:G13))/4</f>
         <v>0.64999999999999991</v>
       </c>
     </row>
@@ -3099,11 +3097,11 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -3115,44 +3113,39 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <f t="shared" ref="H14:H15" si="5">(SUM(D14:G15))/4</f>
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" ref="H14" si="5">(SUM(D14:G15))/4</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H6:H7"/>
@@ -3169,13 +3162,18 @@
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3231,22 +3229,22 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>0.8</v>
       </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14">
-        <v>0</v>
-      </c>
-      <c r="I2" s="14">
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13">
         <f>(SUM(D2:H3))/5</f>
         <v>0.55999999999999994</v>
       </c>
@@ -3261,12 +3259,12 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -3278,23 +3276,23 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="14">
         <v>0.8</v>
       </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14">
-        <v>1</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14">
-        <f t="shared" ref="I4:I15" si="0">(SUM(D4:H5))/5</f>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" ref="I4" si="0">(SUM(D4:H5))/5</f>
         <v>0.96</v>
       </c>
     </row>
@@ -3308,12 +3306,12 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -3325,23 +3323,23 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14">
-        <f t="shared" ref="I6:I15" si="1">(SUM(D6:H7))/5</f>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" ref="I6" si="1">(SUM(D6:H7))/5</f>
         <v>0.6</v>
       </c>
     </row>
@@ -3355,12 +3353,12 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -3372,23 +3370,23 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>0</v>
-      </c>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <f t="shared" ref="I8:I15" si="2">(SUM(D8:H9))/5</f>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" ref="I8" si="2">(SUM(D8:H9))/5</f>
         <v>0.6</v>
       </c>
     </row>
@@ -3402,12 +3400,12 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -3419,23 +3417,23 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14">
-        <f t="shared" ref="I10:I15" si="3">(SUM(D10:H11))/5</f>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" ref="I10" si="3">(SUM(D10:H11))/5</f>
         <v>1</v>
       </c>
     </row>
@@ -3449,12 +3447,12 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -3466,23 +3464,23 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>0.8</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>0.7</v>
       </c>
-      <c r="F12" s="14">
-        <v>1</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <f t="shared" ref="I12:I15" si="4">(SUM(D12:H13))/5</f>
+      <c r="F12" s="13">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" ref="I12" si="4">(SUM(D12:H13))/5</f>
         <v>0.5</v>
       </c>
     </row>
@@ -3496,12 +3494,12 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -3513,42 +3511,60 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <f t="shared" ref="I14:I15" si="5">(SUM(D14:H15))/5</f>
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" ref="I14" si="5">(SUM(D14:H15))/5</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="D12:D13"/>
@@ -3557,34 +3573,16 @@
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3639,22 +3637,22 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>0.7</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>0.7</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <v>0.7</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>0.7</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <v>0.7</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="13">
         <f>(SUM(D2:H3))/5</f>
         <v>0.7</v>
       </c>
@@ -3669,12 +3667,12 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -3686,23 +3684,23 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="14">
         <v>0.6</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>0.7</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>0.7</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>0.7</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>0.7</v>
       </c>
-      <c r="I4" s="14">
-        <f t="shared" ref="I4:I15" si="0">(SUM(D4:H5))/5</f>
+      <c r="I4" s="13">
+        <f t="shared" ref="I4" si="0">(SUM(D4:H5))/5</f>
         <v>0.67999999999999994</v>
       </c>
     </row>
@@ -3716,12 +3714,12 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -3733,23 +3731,23 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14">
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
         <v>0.7</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>0.7</v>
       </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14">
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
         <v>0.7</v>
       </c>
-      <c r="I6" s="14">
-        <f t="shared" ref="I6:I15" si="1">(SUM(D6:H7))/5</f>
+      <c r="I6" s="13">
+        <f t="shared" ref="I6" si="1">(SUM(D6:H7))/5</f>
         <v>0.82</v>
       </c>
     </row>
@@ -3763,12 +3761,12 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -3780,23 +3778,23 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>1</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <f t="shared" ref="I8:I15" si="2">(SUM(D8:H9))/5</f>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" ref="I8" si="2">(SUM(D8:H9))/5</f>
         <v>1</v>
       </c>
     </row>
@@ -3810,12 +3808,12 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -3827,23 +3825,23 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="14">
         <v>0.7</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>0.8</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>0.7</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>0.7</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>0.7</v>
       </c>
-      <c r="I10" s="14">
-        <f t="shared" ref="I10:I15" si="3">(SUM(D10:H11))/5</f>
+      <c r="I10" s="13">
+        <f t="shared" ref="I10" si="3">(SUM(D10:H11))/5</f>
         <v>0.72000000000000008</v>
       </c>
     </row>
@@ -3857,12 +3855,12 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -3874,23 +3872,23 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="13">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <f t="shared" ref="I12:I15" si="4">(SUM(D12:H13))/5</f>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" ref="I12" si="4">(SUM(D12:H13))/5</f>
         <v>0</v>
       </c>
     </row>
@@ -3904,12 +3902,12 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -3921,42 +3919,60 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="13">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <f t="shared" ref="I14:I15" si="5">(SUM(D14:H15))/5</f>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" ref="I14" si="5">(SUM(D14:H15))/5</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="D12:D13"/>
@@ -3965,34 +3981,16 @@
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4003,7 +4001,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K15"/>
+      <selection activeCell="K2" sqref="K2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4053,30 +4051,30 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14">
-        <v>0</v>
-      </c>
-      <c r="I2" s="14">
-        <v>0</v>
-      </c>
-      <c r="J2" s="14">
-        <v>0</v>
-      </c>
-      <c r="K2" s="14">
+      <c r="D2" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="13">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
+        <v>1</v>
+      </c>
+      <c r="K2" s="13">
         <f>(SUM(D2:J3))/7</f>
-        <v>0</v>
+        <v>0.82857142857142851</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -4089,14 +4087,14 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -4108,29 +4106,29 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
-        <v>0</v>
-      </c>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0</v>
-      </c>
-      <c r="I4" s="14">
-        <v>0</v>
-      </c>
-      <c r="J4" s="14">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14">
-        <f t="shared" ref="K4:K15" si="0">(SUM(D4:J5))/7</f>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
+        <f t="shared" ref="K4" si="0">(SUM(D4:J5))/7</f>
         <v>0</v>
       </c>
     </row>
@@ -4144,14 +4142,14 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -4163,29 +4161,29 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14">
-        <v>1</v>
-      </c>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14">
-        <v>0</v>
-      </c>
-      <c r="J6" s="14">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14">
-        <f t="shared" ref="K6:K15" si="1">(SUM(D6:J7))/7</f>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6" si="1">(SUM(D6:J7))/7</f>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -4199,14 +4197,14 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -4218,29 +4216,29 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>1</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="14">
-        <v>1</v>
-      </c>
-      <c r="K8" s="14">
-        <f t="shared" ref="K8:K15" si="2">(SUM(D8:J9))/7</f>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
+        <f t="shared" ref="K8" si="2">(SUM(D8:J9))/7</f>
         <v>1</v>
       </c>
     </row>
@@ -4254,14 +4252,14 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -4273,29 +4271,29 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="14">
-        <v>1</v>
-      </c>
-      <c r="K10" s="14">
-        <f t="shared" ref="K10:K15" si="3">(SUM(D10:J11))/7</f>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13">
+        <v>1</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" ref="K10" si="3">(SUM(D10:J11))/7</f>
         <v>1</v>
       </c>
     </row>
@@ -4309,14 +4307,14 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -4328,29 +4326,29 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
-        <v>1</v>
-      </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
-        <v>1</v>
-      </c>
-      <c r="K12" s="14">
-        <f t="shared" ref="K12:K15" si="4">(SUM(D12:J13))/7</f>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
+        <v>1</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" ref="K12" si="4">(SUM(D12:J13))/7</f>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -4364,14 +4362,14 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -4383,57 +4381,70 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
-        <f t="shared" ref="K14:K15" si="5">(SUM(D14:J15))/7</f>
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" ref="K14" si="5">(SUM(D14:J15))/7</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="D12:D13"/>
@@ -4449,34 +4460,21 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4531,16 +4529,16 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>0.5</v>
       </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14">
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
         <f>(SUM(D2:F3))/3</f>
         <v>0.83333333333333337</v>
       </c>
@@ -4555,10 +4553,10 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -4570,17 +4568,17 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="14">
         <v>0.5</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>0.8</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>0.6</v>
       </c>
-      <c r="G4" s="14">
-        <f t="shared" ref="G4:G15" si="0">(SUM(D4:F5))/3</f>
+      <c r="G4" s="13">
+        <f t="shared" ref="G4" si="0">(SUM(D4:F5))/3</f>
         <v>0.6333333333333333</v>
       </c>
     </row>
@@ -4594,10 +4592,10 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -4609,17 +4607,17 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14">
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
         <v>0.7</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>0.7</v>
       </c>
-      <c r="G6" s="14">
-        <f t="shared" ref="G6:G15" si="1">(SUM(D6:F7))/3</f>
+      <c r="G6" s="13">
+        <f t="shared" ref="G6" si="1">(SUM(D6:F7))/3</f>
         <v>0.79999999999999993</v>
       </c>
     </row>
@@ -4633,10 +4631,10 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -4648,17 +4646,17 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
         <v>0.8</v>
       </c>
-      <c r="F8" s="14">
-        <v>1</v>
-      </c>
-      <c r="G8" s="14">
-        <f t="shared" ref="G8:G15" si="2">(SUM(D8:F9))/3</f>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" ref="G8" si="2">(SUM(D8:F9))/3</f>
         <v>0.93333333333333324</v>
       </c>
     </row>
@@ -4672,10 +4670,10 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -4687,17 +4685,17 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <f t="shared" ref="G10:G15" si="3">(SUM(D10:F11))/3</f>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" ref="G10" si="3">(SUM(D10:F11))/3</f>
         <v>1</v>
       </c>
     </row>
@@ -4711,10 +4709,10 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -4726,17 +4724,17 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>0.7</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>0.5</v>
       </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <f t="shared" ref="G12:G15" si="4">(SUM(D12:F13))/3</f>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" ref="G12" si="4">(SUM(D12:F13))/3</f>
         <v>0.39999999999999997</v>
       </c>
     </row>
@@ -4750,10 +4748,10 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -4765,37 +4763,31 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>0.5</v>
       </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <f t="shared" ref="G14:G15" si="5">(SUM(D14:F15))/3</f>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" ref="G14" si="5">(SUM(D14:F15))/3</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G2:G3"/>
@@ -4812,9 +4804,15 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4876,28 +4874,28 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14">
-        <v>1</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14">
-        <v>1</v>
-      </c>
-      <c r="K2" s="14">
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
+        <v>1</v>
+      </c>
+      <c r="K2" s="13">
         <f>(SUM(D2:J3))/7</f>
         <v>1</v>
       </c>
@@ -4912,14 +4910,14 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -4931,29 +4929,29 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14">
-        <v>1</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="14">
-        <v>1</v>
-      </c>
-      <c r="K4" s="14">
-        <f t="shared" ref="K4:K15" si="0">(SUM(D4:J5))/7</f>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13">
+        <f t="shared" ref="K4" si="0">(SUM(D4:J5))/7</f>
         <v>1</v>
       </c>
     </row>
@@ -4967,14 +4965,14 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -4986,29 +4984,29 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14">
-        <v>1</v>
-      </c>
-      <c r="F6" s="14">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="14">
-        <v>1</v>
-      </c>
-      <c r="K6" s="14">
-        <f t="shared" ref="K6:K15" si="1">(SUM(D6:J7))/7</f>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6" si="1">(SUM(D6:J7))/7</f>
         <v>1</v>
       </c>
     </row>
@@ -5022,14 +5020,14 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -5041,29 +5039,29 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>1</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <v>1</v>
-      </c>
-      <c r="J8" s="14">
-        <v>1</v>
-      </c>
-      <c r="K8" s="14">
-        <f t="shared" ref="K8:K15" si="2">(SUM(D8:J9))/7</f>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
+        <f t="shared" ref="K8" si="2">(SUM(D8:J9))/7</f>
         <v>1</v>
       </c>
     </row>
@@ -5077,14 +5075,14 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -5096,29 +5094,29 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
-        <v>1</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="14">
-        <v>1</v>
-      </c>
-      <c r="K10" s="14">
-        <f t="shared" ref="K10:K15" si="3">(SUM(D10:J11))/7</f>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13">
+        <v>1</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" ref="K10" si="3">(SUM(D10:J11))/7</f>
         <v>1</v>
       </c>
     </row>
@@ -5132,14 +5130,14 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -5151,29 +5149,29 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
-        <v>1</v>
-      </c>
-      <c r="G12" s="14">
-        <v>1</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-      <c r="I12" s="14">
-        <v>1</v>
-      </c>
-      <c r="J12" s="14">
-        <v>1</v>
-      </c>
-      <c r="K12" s="14">
-        <f t="shared" ref="K12:K15" si="4">(SUM(D12:J13))/7</f>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1</v>
+      </c>
+      <c r="I12" s="13">
+        <v>1</v>
+      </c>
+      <c r="J12" s="13">
+        <v>1</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" ref="K12" si="4">(SUM(D12:J13))/7</f>
         <v>1</v>
       </c>
     </row>
@@ -5187,14 +5185,14 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -5206,85 +5204,44 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
-        <f t="shared" ref="K14:K15" si="5">(SUM(D14:J15))/7</f>
+      <c r="D14" s="13">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" ref="K14" si="5">(SUM(D14:J15))/7</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
@@ -5300,6 +5257,47 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5365,25 +5363,25 @@
       <c r="C2" s="3">
         <v>281528</v>
       </c>
-      <c r="D2" s="13">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14">
-        <v>1</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14">
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
         <f>(SUM(D2:I3))/6</f>
         <v>1</v>
       </c>
@@ -5398,13 +5396,13 @@
       <c r="C3" s="6">
         <v>282193</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -5416,26 +5414,26 @@
       <c r="C4" s="3">
         <v>255300</v>
       </c>
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14">
-        <v>1</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14">
-        <v>1</v>
-      </c>
-      <c r="J4" s="14">
-        <f t="shared" ref="J4:J13" si="0">(SUM(D4:I5))/6</f>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <f t="shared" ref="J4" si="0">(SUM(D4:I5))/6</f>
         <v>1</v>
       </c>
     </row>
@@ -5449,13 +5447,13 @@
       <c r="C5" s="6">
         <v>276864</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -5467,26 +5465,26 @@
       <c r="C6" s="3">
         <v>283749</v>
       </c>
-      <c r="D6" s="13">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14">
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="14">
-        <f t="shared" ref="J6:J13" si="1">(SUM(D6:I7))/6</f>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" ref="J6" si="1">(SUM(D6:I7))/6</f>
         <v>0.5</v>
       </c>
     </row>
@@ -5500,13 +5498,13 @@
       <c r="C7" s="6">
         <v>255295</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
@@ -5518,26 +5516,26 @@
       <c r="C8" s="3">
         <v>286761</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
-        <v>1</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14">
-        <v>0</v>
-      </c>
-      <c r="J8" s="14">
-        <f t="shared" ref="J8:J13" si="2">(SUM(D8:I9))/6</f>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <f t="shared" ref="J8" si="2">(SUM(D8:I9))/6</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -5551,13 +5549,13 @@
       <c r="C9" s="6">
         <v>254049</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
@@ -5569,26 +5567,26 @@
       <c r="C10" s="3">
         <v>285609</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>0.5</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>0.5</v>
       </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14">
-        <v>1</v>
-      </c>
-      <c r="J10" s="14">
-        <f t="shared" ref="J10:J13" si="3">(SUM(D10:I11))/6</f>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13">
+        <f t="shared" ref="J10" si="3">(SUM(D10:I11))/6</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -5602,13 +5600,13 @@
       <c r="C11" s="6">
         <v>286945</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
@@ -5620,25 +5618,25 @@
       <c r="C12" s="3">
         <v>276395</v>
       </c>
-      <c r="D12" s="14">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
         <v>0.2</v>
       </c>
-      <c r="G12" s="14">
-        <v>1</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="14">
+      <c r="G12" s="13">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13">
         <f t="shared" ref="J12:J14" si="4">(SUM(D12:I13))/6</f>
         <v>0.53333333333333333</v>
       </c>
@@ -5653,13 +5651,13 @@
       <c r="C13" s="6">
         <v>285489</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
@@ -5671,57 +5669,60 @@
       <c r="C14" s="6">
         <v>246173</v>
       </c>
-      <c r="D14" s="14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
         <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="D8:D9"/>
@@ -5730,30 +5731,27 @@
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="I8:I9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>